<commit_message>
Thu Nov 18 00:52:24 CST 2021
</commit_message>
<xml_diff>
--- a/笔记/CBAP/2. CBAP BABOK v3.0高级商业分析师考证学习计划 v0.1.xlsx
+++ b/笔记/CBAP/2. CBAP BABOK v3.0高级商业分析师考证学习计划 v0.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" activeTab="1"/>
+    <workbookView windowWidth="24800" windowHeight="13180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="5" r:id="rId1"/>
@@ -2289,10 +2289,10 @@
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
     <numFmt numFmtId="177" formatCode="mm/dd/yy;@"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -2369,10 +2369,40 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2384,6 +2414,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -2392,23 +2461,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2422,16 +2476,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2444,32 +2490,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2484,37 +2514,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2579,7 +2579,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2591,19 +2621,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2621,7 +2675,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2633,13 +2711,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2651,37 +2741,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2693,73 +2753,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2939,6 +2939,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2957,8 +2992,17 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2978,15 +3022,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3001,186 +3036,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5244,7 +5244,7 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
@@ -5294,7 +5294,7 @@
       <c r="A3" s="6"/>
       <c r="B3" s="7">
         <f>I67/G67</f>
-        <v>0.115942028985507</v>
+        <v>0.123188405797101</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -5373,7 +5373,7 @@
       <c r="E7" s="18"/>
       <c r="F7" s="45">
         <f t="shared" ref="F7:F64" si="0">I7/G7</f>
-        <v>0.551724137931034</v>
+        <v>0.586206896551724</v>
       </c>
       <c r="G7" s="15">
         <f>SUM(G8:G27)</f>
@@ -5382,11 +5382,11 @@
       <c r="H7" s="46"/>
       <c r="I7" s="15">
         <f>SUM(I8:I27)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J7" s="15">
         <f>G7-I7</f>
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:10">
@@ -5651,13 +5651,15 @@
       <c r="E18" s="24"/>
       <c r="F18" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G18" s="50">
         <v>2</v>
       </c>
       <c r="H18" s="49"/>
-      <c r="I18" s="60"/>
+      <c r="I18" s="60">
+        <v>1</v>
+      </c>
       <c r="J18" s="59"/>
     </row>
     <row r="19" ht="41.75" spans="1:10">
@@ -6760,11 +6762,11 @@
       <c r="H67" s="70"/>
       <c r="I67" s="70">
         <f>SUM(I7,I28,I59,)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J67" s="71">
         <f>SUM(J7:J66)</f>
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -6781,7 +6783,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{ef721d3d-dee9-4010-95be-618d7ee5fa22}</x14:id>
+          <x14:id>{3636c434-882b-4d46-b74b-dcccaf261bed}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -6800,7 +6802,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{a936971c-69e2-45fc-8b78-b5993d286dad}</x14:id>
+          <x14:id>{3c58efc5-3410-47cd-8094-e654779cc893}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -6815,7 +6817,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{ef721d3d-dee9-4010-95be-618d7ee5fa22}">
+          <x14:cfRule type="dataBar" id="{3636c434-882b-4d46-b74b-dcccaf261bed}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -6830,7 +6832,7 @@
           <xm:sqref>B3:G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{a936971c-69e2-45fc-8b78-b5993d286dad}">
+          <x14:cfRule type="dataBar" id="{3c58efc5-3410-47cd-8094-e654779cc893}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
Fri Jan  7 02:24:07 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CBAP/2. CBAP BABOK v3.0高级商业分析师考证学习计划 v0.1.xlsx
+++ b/笔记/CBAP/2. CBAP BABOK v3.0高级商业分析师考证学习计划 v0.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="24800" windowHeight="13180" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="13180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="5" r:id="rId1"/>
@@ -2288,11 +2288,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="177" formatCode="mm/dd/yy;@"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -2384,8 +2384,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2398,16 +2399,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2422,7 +2446,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2430,34 +2453,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2470,14 +2470,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2499,14 +2492,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2579,7 +2579,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2591,25 +2603,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2621,25 +2633,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2657,31 +2681,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2693,43 +2735,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2741,19 +2753,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2975,25 +2975,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3007,17 +2998,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3036,145 +3021,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3216,7 +3216,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="17" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3225,7 +3225,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="17" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="60" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="2" borderId="0" xfId="17" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="4" fillId="2" borderId="0" xfId="17" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="60" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3246,7 +3246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3255,7 +3255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3267,7 +3267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3294,13 +3294,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3324,7 +3324,7 @@
     <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5246,7 +5246,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomLeft" activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.4285714285714" defaultRowHeight="12"/>
@@ -5294,7 +5294,7 @@
       <c r="A3" s="6"/>
       <c r="B3" s="7">
         <f>I67/G67</f>
-        <v>0.123188405797101</v>
+        <v>0.282608695652174</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -5373,7 +5373,7 @@
       <c r="E7" s="18"/>
       <c r="F7" s="45">
         <f t="shared" ref="F7:F64" si="0">I7/G7</f>
-        <v>0.586206896551724</v>
+        <v>0.793103448275862</v>
       </c>
       <c r="G7" s="15">
         <f>SUM(G8:G27)</f>
@@ -5382,11 +5382,11 @@
       <c r="H7" s="46"/>
       <c r="I7" s="15">
         <f>SUM(I8:I27)</f>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J7" s="15">
         <f>G7-I7</f>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:10">
@@ -5628,13 +5628,15 @@
       <c r="E17" s="24"/>
       <c r="F17" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="50">
         <v>4</v>
       </c>
       <c r="H17" s="49"/>
-      <c r="I17" s="60"/>
+      <c r="I17" s="60">
+        <v>4</v>
+      </c>
       <c r="J17" s="59"/>
     </row>
     <row r="18" ht="29.75" spans="1:10">
@@ -5651,14 +5653,14 @@
       <c r="E18" s="24"/>
       <c r="F18" s="45">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G18" s="50">
         <v>2</v>
       </c>
       <c r="H18" s="49"/>
       <c r="I18" s="60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J18" s="59"/>
     </row>
@@ -5676,13 +5678,15 @@
       <c r="E19" s="24"/>
       <c r="F19" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="50">
         <v>1</v>
       </c>
       <c r="H19" s="49"/>
-      <c r="I19" s="60"/>
+      <c r="I19" s="60">
+        <v>1</v>
+      </c>
       <c r="J19" s="59"/>
     </row>
     <row r="20" ht="41.75" spans="1:10">
@@ -5873,7 +5877,7 @@
       <c r="E28" s="18"/>
       <c r="F28" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.363636363636364</v>
       </c>
       <c r="G28" s="29">
         <f>SUM(G29:G48)</f>
@@ -5882,11 +5886,11 @@
       <c r="H28" s="52"/>
       <c r="I28" s="29">
         <f>SUM(I29:I48)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J28" s="29">
         <f>G28-I28</f>
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" ht="29.75" spans="1:10">
@@ -5903,13 +5907,15 @@
       <c r="E29" s="21"/>
       <c r="F29" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="53">
         <v>2</v>
       </c>
       <c r="H29" s="49"/>
-      <c r="I29" s="58"/>
+      <c r="I29" s="58">
+        <v>2</v>
+      </c>
       <c r="J29" s="59"/>
     </row>
     <row r="30" ht="29.75" spans="1:10">
@@ -5926,13 +5932,15 @@
       <c r="E30" s="24"/>
       <c r="F30" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="50">
         <v>2</v>
       </c>
       <c r="H30" s="49"/>
-      <c r="I30" s="60"/>
+      <c r="I30" s="60">
+        <v>2</v>
+      </c>
       <c r="J30" s="59"/>
     </row>
     <row r="31" ht="29.75" spans="1:10">
@@ -5949,13 +5957,15 @@
       <c r="E31" s="24"/>
       <c r="F31" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="50">
         <v>3</v>
       </c>
       <c r="H31" s="49"/>
-      <c r="I31" s="60"/>
+      <c r="I31" s="60">
+        <v>3</v>
+      </c>
       <c r="J31" s="59"/>
     </row>
     <row r="32" ht="15.75" spans="1:10">
@@ -5995,13 +6005,15 @@
       <c r="E33" s="24"/>
       <c r="F33" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="50">
         <v>3</v>
       </c>
       <c r="H33" s="49"/>
-      <c r="I33" s="60"/>
+      <c r="I33" s="60">
+        <v>3</v>
+      </c>
       <c r="J33" s="59"/>
     </row>
     <row r="34" ht="15.75" spans="1:10">
@@ -6041,13 +6053,15 @@
       <c r="E35" s="24"/>
       <c r="F35" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="50">
         <v>3</v>
       </c>
       <c r="H35" s="49"/>
-      <c r="I35" s="60"/>
+      <c r="I35" s="60">
+        <v>3</v>
+      </c>
       <c r="J35" s="59"/>
     </row>
     <row r="36" ht="15.75" spans="1:10">
@@ -6087,13 +6101,15 @@
       <c r="E37" s="24"/>
       <c r="F37" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="50">
         <v>3</v>
       </c>
       <c r="H37" s="49"/>
-      <c r="I37" s="60"/>
+      <c r="I37" s="60">
+        <v>3</v>
+      </c>
       <c r="J37" s="59"/>
     </row>
     <row r="38" ht="15.75" spans="1:10">
@@ -6762,11 +6778,11 @@
       <c r="H67" s="70"/>
       <c r="I67" s="70">
         <f>SUM(I7,I28,I59,)</f>
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="J67" s="71">
         <f>SUM(J7:J66)</f>
-        <v>121</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -6783,7 +6799,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3636c434-882b-4d46-b74b-dcccaf261bed}</x14:id>
+          <x14:id>{a3563440-7547-4383-ad06-b6239512882f}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -6802,7 +6818,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3c58efc5-3410-47cd-8094-e654779cc893}</x14:id>
+          <x14:id>{86dd7347-0aef-4592-9f7a-e56cf399bbe9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -6817,7 +6833,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3636c434-882b-4d46-b74b-dcccaf261bed}">
+          <x14:cfRule type="dataBar" id="{a3563440-7547-4383-ad06-b6239512882f}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -6832,7 +6848,7 @@
           <xm:sqref>B3:G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3c58efc5-3410-47cd-8094-e654779cc893}">
+          <x14:cfRule type="dataBar" id="{86dd7347-0aef-4592-9f7a-e56cf399bbe9}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
Sun Feb 13 13:21:25 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CBAP/2. CBAP BABOK v3.0高级商业分析师考证学习计划 v0.1.xlsx
+++ b/笔记/CBAP/2. CBAP BABOK v3.0高级商业分析师考证学习计划 v0.1.xlsx
@@ -2288,11 +2288,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -2380,7 +2380,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2393,14 +2400,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2414,17 +2422,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2432,6 +2438,51 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2446,60 +2497,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2513,10 +2513,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2579,7 +2579,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2591,43 +2729,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2639,43 +2741,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2693,73 +2759,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2954,26 +2954,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2989,20 +2969,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3022,162 +2999,185 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3216,7 +3216,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="17" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3225,7 +3225,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="17" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="60" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="2" borderId="0" xfId="17" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="2" borderId="0" xfId="17" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="60" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3246,7 +3246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3255,7 +3255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3267,7 +3267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3294,13 +3294,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3324,7 +3324,7 @@
     <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5244,9 +5244,9 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J38" sqref="J38"/>
+      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.4285714285714" defaultRowHeight="12"/>
@@ -5294,7 +5294,7 @@
       <c r="A3" s="6"/>
       <c r="B3" s="7">
         <f>I67/G67</f>
-        <v>0.282608695652174</v>
+        <v>0.376811594202899</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -5877,7 +5877,7 @@
       <c r="E28" s="18"/>
       <c r="F28" s="45">
         <f t="shared" si="0"/>
-        <v>0.363636363636364</v>
+        <v>0.659090909090909</v>
       </c>
       <c r="G28" s="29">
         <f>SUM(G29:G48)</f>
@@ -5886,11 +5886,11 @@
       <c r="H28" s="52"/>
       <c r="I28" s="29">
         <f>SUM(I29:I48)</f>
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="J28" s="29">
         <f>G28-I28</f>
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" ht="29.75" spans="1:10">
@@ -6149,13 +6149,15 @@
       <c r="E39" s="24"/>
       <c r="F39" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="50">
         <v>4</v>
       </c>
       <c r="H39" s="49"/>
-      <c r="I39" s="60"/>
+      <c r="I39" s="60">
+        <v>4</v>
+      </c>
       <c r="J39" s="59"/>
     </row>
     <row r="40" ht="15.75" spans="1:10">
@@ -6195,13 +6197,15 @@
       <c r="E41" s="24"/>
       <c r="F41" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="50">
         <v>3</v>
       </c>
       <c r="H41" s="49"/>
-      <c r="I41" s="60"/>
+      <c r="I41" s="60">
+        <v>3</v>
+      </c>
       <c r="J41" s="59"/>
     </row>
     <row r="42" ht="15.75" spans="1:10">
@@ -6241,13 +6245,15 @@
       <c r="E43" s="24"/>
       <c r="F43" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="50">
         <v>6</v>
       </c>
       <c r="H43" s="49"/>
-      <c r="I43" s="60"/>
+      <c r="I43" s="60">
+        <v>6</v>
+      </c>
       <c r="J43" s="59"/>
     </row>
     <row r="44" ht="15.75" spans="1:10">
@@ -6778,11 +6784,11 @@
       <c r="H67" s="70"/>
       <c r="I67" s="70">
         <f>SUM(I7,I28,I59,)</f>
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="J67" s="71">
         <f>SUM(J7:J66)</f>
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -6799,7 +6805,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{a3563440-7547-4383-ad06-b6239512882f}</x14:id>
+          <x14:id>{f5d07601-4fc6-451b-aebd-395ff8bef819}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -6818,7 +6824,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{86dd7347-0aef-4592-9f7a-e56cf399bbe9}</x14:id>
+          <x14:id>{833e6a1c-50a0-4d44-82bf-e105f5bee9b9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -6833,7 +6839,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{a3563440-7547-4383-ad06-b6239512882f}">
+          <x14:cfRule type="dataBar" id="{f5d07601-4fc6-451b-aebd-395ff8bef819}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -6848,7 +6854,7 @@
           <xm:sqref>B3:G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{86dd7347-0aef-4592-9f7a-e56cf399bbe9}">
+          <x14:cfRule type="dataBar" id="{833e6a1c-50a0-4d44-82bf-e105f5bee9b9}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>